<commit_message>
my test commit message.
</commit_message>
<xml_diff>
--- a/testSourceOfTruth.xlsx
+++ b/testSourceOfTruth.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salvatore.Servodio\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofdelaware.sharepoint.com/teams/DTIEnterpriseArchitecture/Shared Documents/Innovation Space/Work Space/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE08AB60-4726-4489-95C9-5F9835BD928E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_28F3E28AB5B27A90CF08B69946F8E86C62C08431" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58E7E13C-987B-4F3B-8166-514F26C64B50}"/>
   <bookViews>
     <workbookView xWindow="6375" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,6 +461,25 @@
       </c>
       <c r="C5">
         <v>777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>111</v>
+      </c>
+      <c r="B6">
+        <v>222</v>
+      </c>
+      <c r="C6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>888</v>
+      </c>
+      <c r="B7">
+        <v>9999</v>
       </c>
     </row>
   </sheetData>
@@ -754,15 +773,15 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4447CDFF-D864-49DA-974A-09DB13BB16D9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8c426987-cbfe-4caf-9048-eb83e867e586"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8c426987-cbfe-4caf-9048-eb83e867e586"/>
     <ds:schemaRef ds:uri="621a3a1b-73b8-431c-a0fb-6f5c740eddc3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>